<commit_message>
Changed some visual changes, fixed bug with declining
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Bugs:</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Admins cannot decline apps</t>
+  </si>
+  <si>
+    <t>Apps with "" as name are just blank</t>
+  </si>
+  <si>
+    <t>Yes they are</t>
   </si>
 </sst>
 </file>
@@ -401,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,6 +523,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug with nil apps in AppController
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Bugs:</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Yes they are</t>
+  </si>
+  <si>
+    <t>Website will crash if try to delete nil app</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,6 +534,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>